<commit_message>
added comments to random number gen
</commit_message>
<xml_diff>
--- a/144F20/Topic 4/PayingMinOnCC.xlsx
+++ b/144F20/Topic 4/PayingMinOnCC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{F68BCEB6-314B-4768-917A-4943007F4DD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ECC0DB-1FB3-44CD-AC80-8EAFF891866D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="19530" windowHeight="14385" xr2:uid="{CF10E6CE-D87B-417F-86FF-EEF4FA94E14B}"/>
   </bookViews>
@@ -293,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -681,6 +681,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -688,7 +701,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -777,6 +790,16 @@
     <xf numFmtId="43" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -940,6 +963,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1007,9 +1035,440 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1577868" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25915002-C696-4193-B9C4-1FDDF7836A99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085850" y="657225"/>
+          <a:ext cx="1577868" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>This generates the seed.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1554785" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{956AF120-D35B-4849-89C0-AD367211F635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3171825" y="38100"/>
+          <a:ext cx="1554785" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>A table of some primes!</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3319755" cy="953466"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3A6186E-FA44-4037-B073-FB475FA9E4DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="4467225"/>
+          <a:ext cx="3319755" cy="953466"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The actual formula:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    next = mod((current)*1103515245 +  12345, 32768)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The first value of "current" is "seed"</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>143358</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9484C0E0-B774-4A35-BD32-DBEB2209CFE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1181100" y="2276475"/>
+          <a:ext cx="2781300" cy="2667483"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3218445" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E70F92A-BB9E-4243-94A5-6F13272AE79D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="5667375"/>
+          <a:ext cx="3218445" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Turn</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> the random int into a number between 0 and 1.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>46555</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B24BA5B-9C8B-472C-94E0-DDA07D4E0C87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2381250" y="2266950"/>
+          <a:ext cx="1590675" cy="3532705"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B7F2704E-3800-456D-9EAB-F36BA14F9B15}">
-  <header guid="{B7F2704E-3800-456D-9EAB-F36BA14F9B15}" dateTime="2021-05-13T15:58:43" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C8874410-06D2-46AE-A3FB-993C78445DF3}">
+  <header guid="{C8874410-06D2-46AE-A3FB-993C78445DF3}" dateTime="2021-12-15T14:11:13" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1023,9 +1482,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{B7F2704E-3800-456D-9EAB-F36BA14F9B15}" name="Richard Ketchersid" id="-1739567592" dateTime="2021-05-13T15:58:43"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1328,7 +1785,7 @@
   <dimension ref="A1:M298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1341,38 +1798,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1" thickBot="1">
-      <c r="A1" s="46" t="str">
+      <c r="A1" s="56" t="str">
         <f>IF(C8="Your Name Here!", "Enter your name below.","See how long it takes to pay off $"&amp;Random!H19&amp;" credit card debt paying the minimal payment which is the maximum of "&amp;Random!H20&amp;"% or $"&amp;Random!H22&amp;". The credit card has "&amp;Random!H21&amp;"% APR compounded monthly. You want to find out how long it takes you to pay this off and how much you end up paying. Assume you make your payment on the current balance at the beginnig of each period (month), before interest is acrued.")</f>
         <v>Enter your name below.</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="I2" s="35" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="I2" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="36"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
       <c r="I3" s="9" t="s">
         <v>14</v>
       </c>
@@ -1381,13 +1838,13 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="61"/>
       <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
@@ -1396,13 +1853,13 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
       <c r="I5" s="13" t="s">
         <v>18</v>
       </c>
@@ -1411,13 +1868,13 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A6" s="52"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="54"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="64"/>
       <c r="I6" s="14" t="s">
         <v>20</v>
       </c>
@@ -1434,100 +1891,100 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="62" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="10" spans="1:13" ht="28.15" customHeight="1" thickBot="1">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="19"/>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="J10" s="65" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="J10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="67"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="77"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="56"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="70"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="52"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="80"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="52"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A15" s="33"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="23"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="45"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="55"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="18" spans="1:12" ht="45.75" thickBot="1">
@@ -1553,11 +2010,11 @@
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
       <c r="J19" s="28"/>
       <c r="L19" s="17"/>
     </row>
@@ -1567,11 +2024,11 @@
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:12">
@@ -3520,10 +3977,10 @@
       <c r="E298" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="j7hY/oNBIjWVtIoQ64yBMLLsvn05JR8b1qTvgkOsoP0BIlupWGJsItClLnh8dCYPB8w1PtPkFItdzF4xxgaYmA==" saltValue="gMZWMdRS8OGkharZFsllFQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <customSheetViews>
     <customSheetView guid="{0C13EE4D-7CE1-4AA1-8E50-FA0088A2A213}">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="C9" sqref="C9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -3567,271 +4024,275 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F4AA2A-DDE8-4188-A353-CC009FC8809D}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="H1">
+      <c r="G1" s="29"/>
+      <c r="H1" s="30">
         <v>1</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="30">
         <v>2</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="30">
         <v>3</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="30">
         <v>4</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="30">
         <v>5</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="30">
         <v>6</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="30">
         <v>7</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="30">
         <v>8</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="30">
         <v>9</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="30">
         <v>10</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="30">
         <v>11</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="30">
         <v>12</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="30">
         <v>13</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="30">
         <v>14</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="30">
         <v>15</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="31">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="G2">
+      <c r="G2" s="32">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="33">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="33">
         <v>3</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="33">
         <v>5</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="33">
         <v>7</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="33">
         <v>11</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="33">
         <v>13</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="33">
         <v>17</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="33">
         <v>19</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="33">
         <v>23</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="33">
         <v>29</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="33">
         <v>947</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="33">
         <v>953</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="33">
         <v>967</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="33">
         <v>971</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="33">
         <v>977</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="34">
         <v>983</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="G3">
+      <c r="G3" s="32">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="33">
         <v>31</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="33">
         <v>37</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="33">
         <v>41</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="33">
         <v>43</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="33">
         <v>47</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="33">
         <v>53</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="33">
         <v>59</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="33">
         <v>61</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="33">
         <v>67</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="33">
         <v>71</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="33">
         <v>991</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="33">
         <v>997</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="33">
         <v>1009</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="33">
         <v>1013</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="33">
         <v>1019</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="34">
         <v>1021</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="G4">
+      <c r="G4" s="32">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="33">
         <v>73</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="33">
         <v>79</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="33">
         <v>83</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="33">
         <v>89</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="33">
         <v>97</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="33">
         <v>101</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="33">
         <v>103</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="33">
         <v>107</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="33">
         <v>109</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="33">
         <v>113</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="33">
         <v>1031</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="33">
         <v>1033</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="33">
         <v>1039</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="33">
         <v>1049</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="33">
         <v>1051</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="34">
         <v>1061</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="G5">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1">
+      <c r="G5" s="32">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="33">
         <v>127</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="33">
         <v>131</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="33">
         <v>137</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="33">
         <v>139</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="33">
         <v>149</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="33">
         <v>151</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="33">
         <v>157</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="33">
         <v>163</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="33">
         <v>167</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="33">
         <v>173</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="33">
         <v>1993</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="33">
         <v>1997</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="33">
         <v>1999</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="33">
         <v>2003</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="33">
         <v>2011</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="34">
         <v>2017</v>
       </c>
     </row>
@@ -3839,71 +4300,71 @@
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="29">
         <f>CODE(MID(PayoffCC!C$8,A6,1))</f>
         <v>89</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="30">
         <f>MOD(B6,16)</f>
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="30">
         <f>MOD((B6-C6)/16,16)</f>
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="31">
         <f ca="1">INDIRECT("R"&amp;(C6+1)&amp;"C"&amp;(D6+7),0)</f>
         <v>439</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="32">
         <v>5</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="33">
         <v>179</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="33">
         <v>181</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="33">
         <v>191</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="33">
         <v>193</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="33">
         <v>197</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="33">
         <v>199</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="33">
         <v>211</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="33">
         <v>223</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="33">
         <v>227</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="33">
         <v>229</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="33">
         <v>2063</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="33">
         <v>2069</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="33">
         <v>2081</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="33">
         <v>2083</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="33">
         <v>2087</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="34">
         <v>2089</v>
       </c>
     </row>
@@ -3911,71 +4372,71 @@
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="32">
         <f>CODE(MID(PayoffCC!C$8,A7,1))</f>
         <v>111</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="33">
         <f t="shared" ref="C7:C10" si="0">MOD(B7,16)</f>
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="33">
         <f t="shared" ref="D7:D10" si="1">MOD((B7-C7)/16,16)</f>
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="34">
         <f t="shared" ref="E7:E10" ca="1" si="2">INDIRECT("R"&amp;(C7+1)&amp;"C"&amp;(D7+7),0)</f>
         <v>839</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="32">
         <v>6</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="33">
         <v>233</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="33">
         <v>239</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="33">
         <v>241</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="33">
         <v>251</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="33">
         <v>257</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="33">
         <v>263</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="33">
         <v>269</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="33">
         <v>271</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="33">
         <v>277</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="33">
         <v>281</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="33">
         <v>2131</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="33">
         <v>2137</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="33">
         <v>2141</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="33">
         <v>2143</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="33">
         <v>2153</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="34">
         <v>2161</v>
       </c>
     </row>
@@ -3983,71 +4444,71 @@
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="32">
         <f>CODE(MID(PayoffCC!C$8,A8,1))</f>
         <v>117</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="33">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="34">
         <f t="shared" ca="1" si="2"/>
         <v>211</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="32">
         <v>7</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="33">
         <v>283</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="33">
         <v>293</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="33">
         <v>307</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="33">
         <v>311</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="33">
         <v>313</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="33">
         <v>317</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="33">
         <v>331</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="33">
         <v>337</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="33">
         <v>347</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="33">
         <v>349</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="33">
         <v>2221</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="33">
         <v>2237</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="33">
         <v>2239</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="33">
         <v>2243</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="33">
         <v>2251</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="34">
         <v>2267</v>
       </c>
     </row>
@@ -4055,206 +4516,206 @@
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="32">
         <f>CODE(MID(PayoffCC!C$8,A9,1))</f>
         <v>114</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="33">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="34">
         <f t="shared" ca="1" si="2"/>
         <v>59</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="32">
         <v>8</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="33">
         <v>353</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="33">
         <v>359</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="33">
         <v>367</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="33">
         <v>373</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="33">
         <v>379</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="33">
         <v>383</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="33">
         <v>389</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="33">
         <v>397</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="33">
         <v>401</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="33">
         <v>409</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="33">
         <v>2293</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="33">
         <v>2297</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="33">
         <v>2309</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="33">
         <v>2311</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="33">
         <v>2333</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="34">
         <v>2339</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" ht="15.75" thickBot="1">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="32">
         <f>CODE(MID(PayoffCC!C$8,A10,1))</f>
         <v>32</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="36">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="37">
         <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="32">
         <v>9</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="33">
         <v>419</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="33">
         <v>421</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="33">
         <v>431</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="33">
         <v>433</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="33">
         <v>439</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="33">
         <v>443</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="33">
         <v>449</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="33">
         <v>457</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="33">
         <v>461</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="33">
         <v>463</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="33">
         <v>2371</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="33">
         <v>2377</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="33">
         <v>2381</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="33">
         <v>2383</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="33">
         <v>2389</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="34">
         <v>2393</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="38">
         <f ca="1">MOD(PRODUCT(E6:E10),F13)</f>
         <v>3778</v>
       </c>
       <c r="F11">
         <v>1103515245</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="32">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="33">
         <v>467</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="33">
         <v>479</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="33">
         <v>487</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="33">
         <v>491</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="33">
         <v>499</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="33">
         <v>503</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="33">
         <v>509</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="33">
         <v>521</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="33">
         <v>523</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="33">
         <v>541</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="33">
         <v>2437</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="33">
         <v>2441</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="33">
         <v>2447</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="33">
         <v>2459</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="33">
         <v>2467</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="34">
         <v>2473</v>
       </c>
     </row>
@@ -4281,55 +4742,55 @@
       <c r="F12">
         <v>12345</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="32">
         <v>11</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="33">
         <v>547</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="33">
         <v>557</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="33">
         <v>563</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="33">
         <v>569</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="33">
         <v>571</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="33">
         <v>577</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="33">
         <v>587</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="33">
         <v>593</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="33">
         <v>599</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="33">
         <v>601</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="33">
         <v>2539</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="33">
         <v>2543</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="33">
         <v>2549</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="33">
         <v>2551</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="33">
         <v>2557</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="34">
         <v>2579</v>
       </c>
     </row>
@@ -4356,55 +4817,55 @@
       <c r="F13">
         <v>32768</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="32">
         <v>12</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="33">
         <v>607</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="33">
         <v>613</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="33">
         <v>617</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="33">
         <v>619</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="33">
         <v>631</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="33">
         <v>641</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="33">
         <v>643</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="33">
         <v>647</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="33">
         <v>653</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="33">
         <v>659</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="33">
         <v>2621</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="33">
         <v>2633</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="33">
         <v>2647</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="33">
         <v>2657</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="33">
         <v>2659</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="34">
         <v>2663</v>
       </c>
     </row>
@@ -4428,55 +4889,55 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="32">
         <v>13</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="33">
         <v>661</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="33">
         <v>673</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="33">
         <v>677</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="33">
         <v>683</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="33">
         <v>691</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="33">
         <v>701</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="33">
         <v>709</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="33">
         <v>719</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="33">
         <v>727</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="33">
         <v>733</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="33">
         <v>2689</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="33">
         <v>2693</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="33">
         <v>2699</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="33">
         <v>2707</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="33">
         <v>2711</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="34">
         <v>2713</v>
       </c>
     </row>
@@ -4500,55 +4961,55 @@
         <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="32">
         <v>14</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="33">
         <v>739</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="33">
         <v>743</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="33">
         <v>751</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="33">
         <v>757</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="33">
         <v>761</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="33">
         <v>769</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="33">
         <v>773</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="33">
         <v>787</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="33">
         <v>797</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="33">
         <v>809</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="33">
         <v>2749</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="33">
         <v>2753</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="33">
         <v>2767</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="33">
         <v>2777</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="33">
         <v>2789</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="34">
         <v>2791</v>
       </c>
     </row>
@@ -4572,59 +5033,59 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="32">
         <v>15</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="33">
         <v>811</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="33">
         <v>821</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="33">
         <v>823</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="33">
         <v>827</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="33">
         <v>829</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="33">
         <v>839</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="33">
         <v>853</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="33">
         <v>857</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="33">
         <v>859</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="33">
         <v>863</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="33">
         <v>2833</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="33">
         <v>2837</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="33">
         <v>2843</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="33">
         <v>2851</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="33">
         <v>2857</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="34">
         <v>2861</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4644,55 +5105,55 @@
         <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="35">
         <v>16</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="36">
         <v>877</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="36">
         <v>881</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="36">
         <v>883</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="36">
         <v>887</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="36">
         <v>907</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="36">
         <v>911</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="36">
         <v>919</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="36">
         <v>929</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="36">
         <v>937</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="36">
         <v>941</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="36">
         <v>2909</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="36">
         <v>2917</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="36">
         <v>2927</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="36">
         <v>2939</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="36">
         <v>2953</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="37">
         <v>2957</v>
       </c>
     </row>
@@ -5062,11 +5523,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0C13EE4D-7CE1-4AA1-8E50-FA0088A2A213}" state="hidden" topLeftCell="A10">
-      <selection activeCell="H21" sqref="H21"/>
+    <customSheetView guid="{0C13EE4D-7CE1-4AA1-8E50-FA0088A2A213}" state="hidden">
+      <selection activeCell="P25" sqref="P25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change C2 to B4
</commit_message>
<xml_diff>
--- a/144F20/Topic 4/PayingMinOnCC.xlsx
+++ b/144F20/Topic 4/PayingMinOnCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="10_ncr:80_{02A4D49E-1BE3-41D5-8229-9ED30F380881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D399125-8318-469B-8C6C-299A7BF42572}"/>
+  <xr:revisionPtr revIDLastSave="358" documentId="10_ncr:80_{02A4D49E-1BE3-41D5-8229-9ED30F380881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A20AE776-9188-47E3-8F3A-1776AF79741C}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="10152" xr2:uid="{CF10E6CE-D87B-417F-86FF-EEF4FA94E14B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF10E6CE-D87B-417F-86FF-EEF4FA94E14B}"/>
   </bookViews>
   <sheets>
     <sheet name="PayingMinPmt" sheetId="1" r:id="rId1"/>
@@ -238,9 +238,6 @@
     <t xml:space="preserve">5) </t>
   </si>
   <si>
-    <t>What is your best guess in C2?</t>
-  </si>
-  <si>
     <t>In this last tab figure out how much you need to pay each month in order to pay off the entire amount in 24 months. (Find this correct to two decimals, K8 should say "Just right" when you have this correct.</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
       </rPr>
       <t>Enter your answers below and reflect on what you notice for part 3 of the project.</t>
     </r>
+  </si>
+  <si>
+    <t>What is your best guess in B4?</t>
   </si>
 </sst>
 </file>
@@ -1187,30 +1187,6 @@
     <xf numFmtId="1" fontId="0" fillId="9" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1355,6 +1331,34 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
@@ -1449,10 +1453,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2374,51 +2374,51 @@
       <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="22"/>
-    <col min="2" max="2" width="10.109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="22"/>
+    <col min="2" max="2" width="10.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="22" customWidth="1"/>
-    <col min="5" max="8" width="8.88671875" style="22"/>
-    <col min="9" max="9" width="16.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.85546875" style="22"/>
+    <col min="9" max="9" width="16.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="22"/>
+    <col min="11" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" customHeight="1" thickBot="1">
-      <c r="A1" s="101" t="str">
+    <row r="1" spans="1:12" ht="14.45" customHeight="1" thickBot="1">
+      <c r="A1" s="95" t="str">
         <f>IF(C10="Your Name Here!", "Enter your name below and your very own problem will appear here:)","Discover both how much is paid and how long it takes to pay off a $"&amp;Random!H19&amp;" credit card debt paying the minimal payment which is the maximum of "&amp;Random!H20&amp;"% or $"&amp;Random!H22&amp;". The credit card has "&amp;Random!H21&amp;"% APR compounded monthly. You want to find out how long it takes you to pay this off and how much you end up paying. Assume you make your payment on the current balance at the beginnig of each period (month), before interest is acrued"&amp;" and assuming that the card is not being used for any additional charges.")</f>
         <v>Enter your name below and your very own problem will appear here:)</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="103"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1">
-      <c r="A2" s="104"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
-      <c r="I2" s="74" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="97"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A2" s="98"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="100"/>
+      <c r="I2" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="75"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1">
-      <c r="A3" s="104"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="106"/>
+      <c r="J2" s="69"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A3" s="98"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="100"/>
       <c r="I3" s="53" t="s">
         <v>13</v>
       </c>
@@ -2427,13 +2427,13 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="104"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="106"/>
+      <c r="A4" s="98"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
       <c r="I4" s="55" t="s">
         <v>52</v>
       </c>
@@ -2442,13 +2442,13 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="104"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="106"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="100"/>
       <c r="I5" s="57" t="s">
         <v>16</v>
       </c>
@@ -2457,13 +2457,13 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="104"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="A6" s="98"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="100"/>
       <c r="I6" s="59" t="s">
         <v>18</v>
       </c>
@@ -2471,14 +2471,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1">
-      <c r="A7" s="104"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="106"/>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A7" s="98"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="100"/>
       <c r="I7" s="60" t="s">
         <v>20</v>
       </c>
@@ -2486,122 +2486,122 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="62" customFormat="1" ht="15" thickBot="1">
-      <c r="A8" s="107"/>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="109"/>
-    </row>
-    <row r="9" spans="1:12" s="62" customFormat="1" ht="15" thickBot="1">
+    <row r="8" spans="1:12" s="62" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A8" s="101"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="103"/>
+    </row>
+    <row r="9" spans="1:12" s="62" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="63"/>
       <c r="B9" s="63"/>
       <c r="C9" s="64"/>
       <c r="D9" s="64"/>
       <c r="E9" s="64"/>
-      <c r="I9" s="95" t="s">
+      <c r="I9" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="97"/>
-    </row>
-    <row r="10" spans="1:12" s="62" customFormat="1" ht="15" thickBot="1">
-      <c r="A10" s="90" t="s">
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="91"/>
+    </row>
+    <row r="10" spans="1:12" s="62" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A10" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92" t="s">
+      <c r="B10" s="85"/>
+      <c r="C10" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="93"/>
-      <c r="E10" s="94"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="100"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1"/>
-    <row r="12" spans="1:12" ht="28.2" customHeight="1" thickBot="1">
-      <c r="A12" s="88" t="s">
+      <c r="D10" s="87"/>
+      <c r="E10" s="88"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="94"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:12" ht="28.15" customHeight="1" thickBot="1">
+      <c r="A12" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="89"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="78"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="86"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="81"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
-      <c r="A14" s="87" t="s">
+      <c r="D13" s="73"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="75"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A14" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="86"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="67">
         <v>12</v>
       </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="81"/>
-    </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1">
-      <c r="A15" s="69" t="s">
+      <c r="D14" s="73"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="75"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A15" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="81"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="75"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="72" t="s">
+      <c r="A16" s="108" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="81"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1">
-      <c r="A17" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="75"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A17" s="109"/>
       <c r="B17" s="4"/>
       <c r="C17" s="43"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="84"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1"/>
-    <row r="20" spans="1:12" ht="29.4" thickBot="1">
+      <c r="D17" s="76"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="78"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:12" ht="45.75" thickBot="1">
       <c r="A20" s="29" t="s">
         <v>11</v>
       </c>
@@ -2626,11 +2626,11 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104"/>
       <c r="J21" s="21"/>
       <c r="K21" s="22" t="s">
         <v>53</v>
@@ -2645,11 +2645,11 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:12">
@@ -2660,11 +2660,11 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="G23" s="68" t="s">
+      <c r="G23" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
       <c r="J23" s="66"/>
     </row>
     <row r="24" spans="1:12">
@@ -7141,6 +7141,11 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="14">
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="D12:H17"/>
     <mergeCell ref="A13:B13"/>
@@ -7150,11 +7155,6 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="I9:L10"/>
     <mergeCell ref="A1:G8"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:E10">
     <cfRule type="expression" dxfId="4" priority="2">
@@ -7179,194 +7179,194 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="22"/>
+    <col min="1" max="1" width="8.85546875" style="22"/>
     <col min="2" max="4" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.88671875" style="22"/>
-    <col min="10" max="10" width="12.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="22"/>
+    <col min="5" max="9" width="8.85546875" style="22"/>
+    <col min="10" max="10" width="12.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="89"/>
+      <c r="B1" s="83"/>
       <c r="C1" s="2"/>
-      <c r="F1" s="116" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="118"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
-      <c r="A2" s="85" t="s">
+      <c r="F1" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="119"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A2" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="86"/>
+      <c r="B2" s="80"/>
       <c r="C2" s="3"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="121"/>
-    </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="F2" s="120"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="122"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="80"/>
       <c r="C3" s="41">
         <v>12</v>
       </c>
-      <c r="F3" s="119"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
-      <c r="O3" s="120"/>
-      <c r="P3" s="120"/>
-      <c r="Q3" s="120"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="121"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
-      <c r="A4" s="69" t="s">
+      <c r="F3" s="120"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="121"/>
+      <c r="O3" s="121"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" s="121"/>
+      <c r="S3" s="122"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="71"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="121"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="122"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="110" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="119"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="120"/>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="121"/>
-    </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
-      <c r="A6" s="73"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="122"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A6" s="109"/>
       <c r="B6" s="4"/>
       <c r="C6" s="43"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="120"/>
-      <c r="O6" s="120"/>
-      <c r="P6" s="120"/>
-      <c r="Q6" s="120"/>
-      <c r="R6" s="120"/>
-      <c r="S6" s="121"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="122"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="F7" s="119"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="120"/>
-      <c r="N7" s="120"/>
-      <c r="O7" s="120"/>
-      <c r="P7" s="120"/>
-      <c r="Q7" s="120"/>
-      <c r="R7" s="120"/>
-      <c r="S7" s="121"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
+      <c r="R7" s="121"/>
+      <c r="S7" s="122"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="F8" s="119"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="120"/>
-      <c r="O8" s="120"/>
-      <c r="P8" s="120"/>
-      <c r="Q8" s="120"/>
-      <c r="R8" s="120"/>
-      <c r="S8" s="121"/>
-    </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
-      <c r="F9" s="119"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
-      <c r="O9" s="120"/>
-      <c r="P9" s="120"/>
-      <c r="Q9" s="120"/>
-      <c r="R9" s="120"/>
-      <c r="S9" s="121"/>
-    </row>
-    <row r="10" spans="1:19" ht="43.8" thickBot="1">
+      <c r="F8" s="120"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="121"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="122"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1">
+      <c r="F9" s="120"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="122"/>
+    </row>
+    <row r="10" spans="1:19" ht="45.75" thickBot="1">
       <c r="A10" s="29" t="s">
         <v>11</v>
       </c>
@@ -7382,20 +7382,20 @@
       <c r="E10" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="123"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="123"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="124"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="124"/>
+      <c r="O10" s="124"/>
+      <c r="P10" s="124"/>
+      <c r="Q10" s="124"/>
+      <c r="R10" s="124"/>
+      <c r="S10" s="125"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="33">
@@ -7417,11 +7417,11 @@
         <f>IF(OR($C$1="",$C$2="",$C$3="",$B$5="",$B$6="",D11=""),"",D11*C$1/C$3)</f>
         <v/>
       </c>
-      <c r="G11" s="133" t="s">
+      <c r="G11" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
       <c r="J11" s="44" t="str">
         <f>IF(B509&lt;&gt;"",(COUNTIF(D11:D509,"&lt;&gt;0")+1)/12,"")</f>
         <v/>
@@ -7450,11 +7450,11 @@
         <f>IF(OR($C$1="",$C$2="",$C$3="",$B$5="",$B$6="",D12=""),"",D12*C$1/C$3)</f>
         <v/>
       </c>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="104"/>
       <c r="J12" s="46" t="str">
         <f>IF(B509&lt;&gt;"",SUM(C11:C509),"")</f>
         <v/>
@@ -7480,17 +7480,17 @@
         <f>IF(OR($C$1="",$C$2="",$C$3="",$B$5="",$B$6="",D13=""),"",D13*C$1/C$3)</f>
         <v/>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="G13" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
       <c r="J13" s="47" t="str">
         <f>IF(B509&lt;&gt;"",J12-C2,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" thickBot="1">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1">
       <c r="A14" s="33">
         <v>4</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1">
+    <row r="15" spans="1:19" ht="15.75" thickBot="1">
       <c r="A15" s="33">
         <v>5</v>
       </c>
@@ -7532,13 +7532,13 @@
         <v/>
       </c>
       <c r="G15" s="52"/>
-      <c r="H15" s="113" t="s">
+      <c r="H15" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="114"/>
-      <c r="J15" s="114"/>
-      <c r="K15" s="114"/>
-      <c r="L15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="116"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="33">
@@ -7563,11 +7563,11 @@
       <c r="G16" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="125"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="126"/>
-      <c r="K16" s="126"/>
-      <c r="L16" s="127"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="128"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="33">
@@ -7589,11 +7589,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H17" s="128"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
-      <c r="K17" s="129"/>
-      <c r="L17" s="130"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
+      <c r="K17" s="130"/>
+      <c r="L17" s="131"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="33">
@@ -7615,11 +7615,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H18" s="128"/>
-      <c r="I18" s="129"/>
-      <c r="J18" s="129"/>
-      <c r="K18" s="129"/>
-      <c r="L18" s="130"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="130"/>
+      <c r="L18" s="131"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="33">
@@ -7644,11 +7644,11 @@
       <c r="G19" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="110"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="132"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="133"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="33">
@@ -7673,13 +7673,13 @@
       <c r="G20" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="110"/>
-      <c r="I20" s="131"/>
-      <c r="J20" s="131"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="132"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1">
+      <c r="H20" s="111"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="132"/>
+      <c r="L20" s="133"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" s="33">
         <v>11</v>
       </c>
@@ -7702,13 +7702,13 @@
       <c r="G21" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="110"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="112"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
+      <c r="H21" s="111"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="113"/>
+    </row>
+    <row r="22" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="33">
         <v>12</v>
       </c>
@@ -7737,7 +7737,7 @@
       <c r="K22" s="50"/>
       <c r="L22" s="50"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickTop="1">
+    <row r="23" spans="1:12" ht="15.75" thickTop="1">
       <c r="A23" s="33">
         <v>13</v>
       </c>
@@ -17967,11 +17967,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="1LKPwXZGaNR4XwwCL8CHOjf/z90Tv44OKUtKoNNu4zjbsJ5ZBN+3/T1gEyJ/wkedoI05t1cPBh/qblKMj6eMKQ==" saltValue="m6GizUWUwaXIqdzikh5KhQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="H21:L21"/>
     <mergeCell ref="H15:L15"/>
     <mergeCell ref="F1:S10"/>
@@ -17981,6 +17976,11 @@
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:J12 F13 A1:C6 F14:I14 F22:I509 F1 A7:E10 F15:G15 F16:H16 F17:F21 H19:H21 G19:G22">
     <cfRule type="expression" dxfId="3" priority="2">
@@ -18001,14 +18001,16 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="8.88671875" style="22"/>
-    <col min="11" max="11" width="9.88671875" style="22" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="22"/>
+    <col min="1" max="8" width="8.85546875" style="22"/>
+    <col min="9" max="9" width="9.5703125" style="22" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="22"/>
+    <col min="11" max="11" width="9.85546875" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -18017,15 +18019,15 @@
       </c>
       <c r="B1" s="143"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="117" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="118"/>
+      <c r="D1" s="118" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="144" t="s">
@@ -18033,15 +18035,15 @@
       </c>
       <c r="B2" s="145"/>
       <c r="C2" s="18"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="121"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1">
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="122"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="146" t="s">
         <v>50</v>
       </c>
@@ -18049,36 +18051,36 @@
       <c r="C3" s="23">
         <v>12</v>
       </c>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="121"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1">
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="122"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1">
       <c r="A4" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="125"/>
     </row>
     <row r="5" spans="1:11">
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1">
       <c r="G6" s="27"/>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="43.8" thickBot="1">
+    <row r="7" spans="1:11" ht="45.75" thickBot="1">
       <c r="A7" s="29" t="s">
         <v>11</v>
       </c>
@@ -18129,7 +18131,7 @@
         <v>Enter PMT</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="33">
         <v>2</v>
       </c>
@@ -18159,7 +18161,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="33">
         <v>3</v>
       </c>
@@ -18180,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
       <c r="A11" s="33">
         <v>4</v>
       </c>
@@ -18201,7 +18203,7 @@
         <v/>
       </c>
       <c r="G11" s="135" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H11" s="136"/>
       <c r="I11" s="137"/>
@@ -18641,7 +18643,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kbbv0/wPNYqWO2YL/0K7wVC0ACOzWbcNoW0T0I0w/wFga9gBM8jTnyAPwk8kMofbCy3IjiqoIG0JF8Kk9vxfBA==" saltValue="QLzcs8tLMpiqgh7XFQWb8A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7Lp55eCRVchAISAEyI+TWqc/Nh3/SZe402JR7yJi7K91EVdKORyu0y0zbw+qt7AzAOV5zxc/ieGClhqvNsDEQQ==" saltValue="NgzGdA/O8LspW24hODjBJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="G8:I8"/>
@@ -18673,7 +18675,7 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -18888,7 +18890,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1">
       <c r="G5" s="10">
         <v>4</v>
       </c>
@@ -19229,7 +19231,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" thickBot="1">
+    <row r="10" spans="1:23" ht="15.75" thickBot="1">
       <c r="A10">
         <v>5</v>
       </c>
@@ -19301,7 +19303,7 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -19730,7 +19732,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15" thickBot="1">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -20186,7 +20188,7 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="2:7">
       <c r="B3" s="147" t="s">

</xml_diff>